<commit_message>
good accuracy of depth
</commit_message>
<xml_diff>
--- a/2.Distance Measurement/output_data.xlsx
+++ b/2.Distance Measurement/output_data.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -359,306 +359,314 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="n">
-        <v>1.25</v>
+        <v>3.73</v>
       </c>
       <c r="B1" t="n">
-        <v>0.5466579861111112</v>
+        <v>0.1244032118055556</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="n">
-        <v>1.25</v>
+        <v>3.28</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5437282986111112</v>
+        <v>0.1709526909722222</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="n">
-        <v>1.59</v>
+        <v>4.62</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4398871527777778</v>
+        <v>0.04584418402777778</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="n">
-        <v>3.95</v>
+        <v>3.88</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1040581597222222</v>
+        <v>0.1103515625</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="n">
-        <v>4.07</v>
+        <v>3.13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.09309895833333333</v>
+        <v>0.1886393229166667</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="n">
-        <v>4.13</v>
+        <v>2.83</v>
       </c>
       <c r="B6" t="n">
-        <v>0.08778211805555555</v>
+        <v>0.2251519097222222</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="n">
-        <v>1.19</v>
+        <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5703125</v>
+        <v>0.2038845486111111</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="n">
-        <v>1.38</v>
+        <v>5.14</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5001627604166666</v>
+        <v>0.006076388888888889</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="n">
-        <v>1.38</v>
+        <v>5.22</v>
       </c>
       <c r="B9" t="n">
-        <v>0.4986436631944444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="n">
-        <v>0.96</v>
+        <v>4.79</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6959092881944444</v>
+        <v>0.03255208333333334</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="n">
-        <v>0.98</v>
+        <v>3.41</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6790907118055556</v>
+        <v>0.1571723090277778</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="n">
-        <v>0.98</v>
+        <v>3.25</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6808810763888888</v>
+        <v>0.1745876736111111</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="n">
-        <v>1.8</v>
+        <v>3.75</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3908962673611111</v>
+        <v>0.1227756076388889</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="n">
-        <v>1.19</v>
+        <v>3.29</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5687934027777778</v>
+        <v>0.1706271701388889</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="n">
-        <v>4.42</v>
+        <v>4.02</v>
       </c>
       <c r="B15" t="n">
-        <v>0.06228298611111111</v>
+        <v>0.09727647569444445</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="n">
-        <v>4.35</v>
+        <v>4.33</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0680881076388889</v>
+        <v>0.07042100694444445</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="n">
-        <v>4.41</v>
+        <v>4.27</v>
       </c>
       <c r="B17" t="n">
-        <v>0.06293402777777778</v>
+        <v>0.0749782986111111</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="n">
-        <v>4.48</v>
+        <v>4.32</v>
       </c>
       <c r="B18" t="n">
-        <v>0.05767144097222222</v>
+        <v>0.07118055555555555</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="n">
-        <v>3.66</v>
+        <v>4.3</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1316731770833333</v>
+        <v>0.07275390625</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="n">
-        <v>3.89</v>
+        <v>4.32</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1092122395833333</v>
+        <v>0.0712890625</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="n">
-        <v>5</v>
+        <v>2.17</v>
       </c>
       <c r="B21" t="n">
-        <v>0.01633029513888889</v>
+        <v>0.3213975694444444</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="n">
-        <v>4.05</v>
+        <v>2.04</v>
       </c>
       <c r="B22" t="n">
-        <v>0.09505208333333333</v>
+        <v>0.3438042534722222</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="n">
-        <v>4.41</v>
+        <v>4.99</v>
       </c>
       <c r="B23" t="n">
-        <v>0.06304253472222222</v>
+        <v>0.01746961805555556</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="n">
-        <v>4.41</v>
+        <v>5.22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.06342230902777778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="n">
-        <v>4.41</v>
+        <v>5.22</v>
       </c>
       <c r="B25" t="n">
-        <v>0.06293402777777778</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="n">
-        <v>2.95</v>
+        <v>5.22</v>
       </c>
       <c r="B26" t="n">
-        <v>0.2090386284722222</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="n">
-        <v>2.96</v>
+        <v>4.86</v>
       </c>
       <c r="B27" t="n">
-        <v>0.2082248263888889</v>
+        <v>0.02674696180555556</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="n">
-        <v>2.99</v>
+        <v>5.33</v>
       </c>
       <c r="B28" t="n">
-        <v>0.2047526041666667</v>
+        <v>-0.0078125</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="n">
-        <v>3.37</v>
+        <v>5.33</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1620008680555556</v>
+        <v>-0.0078125</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="n">
-        <v>3.35</v>
+        <v>5.33</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1636827256944444</v>
+        <v>-0.0078125</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="n">
-        <v>3.02</v>
+        <v>5.33</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2015516493055556</v>
+        <v>-0.0078125</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="n">
-        <v>2.99</v>
+        <v>4.22</v>
       </c>
       <c r="B32" t="n">
-        <v>0.2048611111111111</v>
+        <v>0.07953559027777778</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="n">
-        <v>3.24</v>
+        <v>4.23</v>
       </c>
       <c r="B33" t="n">
-        <v>0.1754014756944444</v>
+        <v>0.07893880208333333</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="n">
-        <v>0.67</v>
+        <v>4.24</v>
       </c>
       <c r="B34" t="n">
-        <v>0.9564344618055556</v>
+        <v>0.07747395833333333</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="n">
-        <v>4.11</v>
+        <v>4.27</v>
       </c>
       <c r="B35" t="n">
-        <v>0.08919270833333333</v>
+        <v>0.0751953125</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="n">
-        <v>4.09</v>
+        <v>4.28</v>
       </c>
       <c r="B36" t="n">
-        <v>0.09147135416666667</v>
+        <v>0.07416449652777778</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="n">
-        <v>0.77</v>
+        <v>4.3</v>
       </c>
       <c r="B37" t="n">
-        <v>0.8718532986111112</v>
+        <v>0.07242838541666667</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="n">
-        <v>4.06</v>
+        <v>4.3</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0935329861111111</v>
+        <v>0.072265625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.08295355902777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
high resolution test on laptop
</commit_message>
<xml_diff>
--- a/2.Distance Measurement/output_data.xlsx
+++ b/2.Distance Measurement/output_data.xlsx
@@ -349,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -359,314 +359,490 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="n">
-        <v>3.73</v>
+        <v>1.84</v>
       </c>
       <c r="B1" t="n">
-        <v>0.1244032118055556</v>
+        <v>0.3834092881944444</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="n">
-        <v>3.28</v>
+        <v>1.17</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1709526909722222</v>
+        <v>0.5770399305555556</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="n">
-        <v>4.62</v>
+        <v>1.35</v>
       </c>
       <c r="B3" t="n">
-        <v>0.04584418402777778</v>
+        <v>0.5110134548611112</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="n">
-        <v>3.88</v>
+        <v>2.47</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1103515625</v>
+        <v>0.2734375</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="n">
-        <v>3.13</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1886393229166667</v>
+        <v>0.9430338541666666</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="n">
-        <v>2.83</v>
+        <v>0.65</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2251519097222222</v>
+        <v>0.9764539930555556</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>2.28</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2038845486111111</v>
+        <v>0.3023003472222222</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="n">
-        <v>5.14</v>
+        <v>4.09</v>
       </c>
       <c r="B8" t="n">
-        <v>0.006076388888888889</v>
+        <v>0.09136284722222222</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="n">
-        <v>5.22</v>
+        <v>1.08</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>0.6234266493055556</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="n">
-        <v>4.79</v>
+        <v>2.81</v>
       </c>
       <c r="B10" t="n">
-        <v>0.03255208333333334</v>
+        <v>0.2265082465277778</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="n">
-        <v>3.41</v>
+        <v>2.88</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1571723090277778</v>
+        <v>0.2183702256944444</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="n">
-        <v>3.25</v>
+        <v>2.87</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1745876736111111</v>
+        <v>0.2192925347222222</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="n">
-        <v>3.75</v>
+        <v>2.83</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1227756076388889</v>
+        <v>0.2242838541666667</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="n">
-        <v>3.29</v>
+        <v>2.84</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1706271701388889</v>
+        <v>0.2235243055555556</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="n">
-        <v>4.02</v>
+        <v>2.83</v>
       </c>
       <c r="B15" t="n">
-        <v>0.09727647569444445</v>
+        <v>0.2245551215277778</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="n">
-        <v>4.33</v>
+        <v>2.9</v>
       </c>
       <c r="B16" t="n">
-        <v>0.07042100694444445</v>
+        <v>0.2160373263888889</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="n">
-        <v>4.27</v>
+        <v>2.87</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0749782986111111</v>
+        <v>0.2194010416666667</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="n">
-        <v>4.32</v>
+        <v>2.88</v>
       </c>
       <c r="B18" t="n">
-        <v>0.07118055555555555</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="n">
-        <v>4.3</v>
+        <v>2.86</v>
       </c>
       <c r="B19" t="n">
-        <v>0.07275390625</v>
+        <v>0.22119140625</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="n">
-        <v>4.32</v>
+        <v>2.84</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0712890625</v>
+        <v>0.2231987847222222</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="n">
-        <v>2.17</v>
+        <v>2.8</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3213975694444444</v>
+        <v>0.2284071180555556</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="n">
-        <v>2.04</v>
+        <v>2.86</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3438042534722222</v>
+        <v>0.2206488715277778</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="n">
-        <v>4.99</v>
+        <v>2.87</v>
       </c>
       <c r="B23" t="n">
-        <v>0.01746961805555556</v>
+        <v>0.21923828125</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="n">
-        <v>5.22</v>
+        <v>2.85</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>0.2221137152777778</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="n">
-        <v>5.22</v>
+        <v>5.33</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>-0.0078125</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="n">
-        <v>5.22</v>
+        <v>5.33</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>-0.0078125</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="n">
-        <v>4.86</v>
+        <v>1.54</v>
       </c>
       <c r="B27" t="n">
-        <v>0.02674696180555556</v>
+        <v>0.4543728298611111</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="n">
-        <v>5.33</v>
+        <v>5.22</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.0078125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="n">
-        <v>5.33</v>
+        <v>2.39</v>
       </c>
       <c r="B29" t="n">
-        <v>-0.0078125</v>
+        <v>0.2853732638888889</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="n">
-        <v>5.33</v>
+        <v>2.19</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.0078125</v>
+        <v>0.3167860243055556</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="n">
-        <v>5.33</v>
+        <v>0.63</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.0078125</v>
+        <v>0.9921875</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="n">
-        <v>4.22</v>
+        <v>3.23</v>
       </c>
       <c r="B32" t="n">
-        <v>0.07953559027777778</v>
+        <v>0.1764322916666667</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="n">
-        <v>4.23</v>
+        <v>0.63</v>
       </c>
       <c r="B33" t="n">
-        <v>0.07893880208333333</v>
+        <v>0.9921875</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="n">
-        <v>4.24</v>
+        <v>0.63</v>
       </c>
       <c r="B34" t="n">
-        <v>0.07747395833333333</v>
+        <v>0.9921875</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="n">
-        <v>4.27</v>
+        <v>0.63</v>
       </c>
       <c r="B35" t="n">
-        <v>0.0751953125</v>
+        <v>0.9921875</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="n">
-        <v>4.28</v>
+        <v>1.27</v>
       </c>
       <c r="B36" t="n">
-        <v>0.07416449652777778</v>
+        <v>0.53759765625</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="n">
-        <v>4.3</v>
+        <v>1.7</v>
       </c>
       <c r="B37" t="n">
-        <v>0.07242838541666667</v>
+        <v>0.4136827256944444</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="n">
-        <v>4.3</v>
+        <v>2.11</v>
       </c>
       <c r="B38" t="n">
-        <v>0.072265625</v>
+        <v>0.3317057291666667</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="n">
-        <v>4.18</v>
+        <v>1.13</v>
       </c>
       <c r="B39" t="n">
-        <v>0.08295355902777778</v>
+        <v>0.5975477430555556</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.1270073784722222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.5674370659722222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.6704644097222222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.6674262152777778</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.662109375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.6754557291666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.6780056423611112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="n">
+        <v>1</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.6688910590277778</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.6654730902777778</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="n">
+        <v>5.22</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.7210286458333334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.7255316840277778</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.7190212673611112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.8559027777777778</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.8513454861111112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.7976345486111112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.1841362847222222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.8272026909722222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.8484700520833334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.8336046006944444</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.8463541666666666</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.8326822916666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>